<commit_message>
2683 +/- 15 Elo at bullet chess.
</commit_message>
<xml_diff>
--- a/LateMoveReductions.xlsx
+++ b/LateMoveReductions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\Documents\Visual Studio 2022\Projects\MadChess\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD045B1-43D7-4C79-B337-C7F96D184120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{547AC38E-B4E8-4D7E-99D0-B2D0F6417ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="1790" windowWidth="28570" windowHeight="18290" xr2:uid="{54AF08ED-B925-40E7-8CD1-F6DF56EC4DEE}"/>
   </bookViews>
@@ -62,18 +62,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -88,13 +82,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -414,299 +407,302 @@
   <dimension ref="A1:BP132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="16384" width="8.7265625" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="2">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="2">
         <v>-96</v>
       </c>
     </row>
     <row r="4" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4">
+      <c r="D4" s="4"/>
+      <c r="E4" s="2">
         <v>1</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <f>E4 + 1</f>
         <v>2</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <f>F4 + 1</f>
         <v>3</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <f>G4 + 1</f>
         <v>4</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="2">
         <f t="shared" ref="I4:BP4" si="0">H4 + 1</f>
         <v>5</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="V4">
+      <c r="V4" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="W4">
+      <c r="W4" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="X4">
+      <c r="X4" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="Y4">
+      <c r="Y4" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="Z4">
+      <c r="Z4" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="AA4">
+      <c r="AA4" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="AB4">
+      <c r="AB4" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AC4">
+      <c r="AC4" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="AD4">
+      <c r="AD4" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="AE4">
+      <c r="AE4" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="AF4">
+      <c r="AF4" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="AG4">
+      <c r="AG4" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="AH4">
+      <c r="AH4" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="AI4">
+      <c r="AI4" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AJ4">
+      <c r="AJ4" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="AK4">
+      <c r="AK4" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="AL4">
+      <c r="AL4" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="AM4">
+      <c r="AM4" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="AN4">
+      <c r="AN4" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="AO4">
+      <c r="AO4" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="AP4">
+      <c r="AP4" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="AQ4">
+      <c r="AQ4" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="AR4">
+      <c r="AR4" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="AS4">
+      <c r="AS4" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="AT4">
+      <c r="AT4" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="AU4">
+      <c r="AU4" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="AV4">
+      <c r="AV4" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="AW4">
+      <c r="AW4" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="AX4">
+      <c r="AX4" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="AY4">
+      <c r="AY4" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="AZ4">
+      <c r="AZ4" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="BA4">
+      <c r="BA4" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="BB4">
+      <c r="BB4" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="BC4">
+      <c r="BC4" s="2">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="BD4">
+      <c r="BD4" s="2">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="BE4">
+      <c r="BE4" s="2">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="BF4">
+      <c r="BF4" s="2">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="BG4">
+      <c r="BG4" s="2">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="BH4">
+      <c r="BH4" s="2">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="BI4">
+      <c r="BI4" s="2">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="BJ4">
+      <c r="BJ4" s="2">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="BK4">
+      <c r="BK4" s="2">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="BL4">
+      <c r="BL4" s="2">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="BM4">
+      <c r="BM4" s="2">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="BN4">
+      <c r="BN4" s="2">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="BO4">
+      <c r="BO4" s="2">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="BP4">
+      <c r="BP4" s="2">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="1">
@@ -967,7 +963,7 @@
       </c>
     </row>
     <row r="6" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="D6">
+      <c r="D6" s="2">
         <f>D5 + 1</f>
         <v>2</v>
       </c>
@@ -1229,7 +1225,7 @@
       </c>
     </row>
     <row r="7" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="D7">
+      <c r="D7" s="2">
         <f>D6 + 1</f>
         <v>3</v>
       </c>
@@ -1277,7 +1273,7 @@
         <f t="shared" si="1"/>
         <v>0.96345918417162779</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="1">
         <f t="shared" si="1"/>
         <v>1.0256347281670544</v>
       </c>
@@ -1491,7 +1487,7 @@
       </c>
     </row>
     <row r="8" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="D8">
+      <c r="D8" s="2">
         <f>D7 + 1</f>
         <v>4</v>
       </c>
@@ -1753,7 +1749,7 @@
       </c>
     </row>
     <row r="9" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="D9">
+      <c r="D9" s="2">
         <f t="shared" ref="D9:D72" si="3">D8 + 1</f>
         <v>5</v>
       </c>
@@ -1809,7 +1805,7 @@
         <f t="shared" si="4"/>
         <v>1.9350484203090228</v>
       </c>
-      <c r="R9" s="2">
+      <c r="R9" s="1">
         <f t="shared" si="4"/>
         <v>2.0126263627291352</v>
       </c>
@@ -2015,7 +2011,7 @@
       </c>
     </row>
     <row r="10" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="D10">
+      <c r="D10" s="2">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
@@ -2277,7 +2273,7 @@
       </c>
     </row>
     <row r="11" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="D11">
+      <c r="D11" s="2">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
@@ -2313,7 +2309,7 @@
         <f t="shared" si="2"/>
         <v>1.8818952394290038</v>
       </c>
-      <c r="M11" s="3">
+      <c r="M11" s="1">
         <f t="shared" si="2"/>
         <v>2.0309701735476668</v>
       </c>
@@ -2539,7 +2535,7 @@
       </c>
     </row>
     <row r="12" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="D12">
+      <c r="D12" s="2">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
@@ -2801,7 +2797,7 @@
       </c>
     </row>
     <row r="13" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="D13">
+      <c r="D13" s="2">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
@@ -2857,7 +2853,7 @@
         <f t="shared" si="2"/>
         <v>2.9156613683954977</v>
       </c>
-      <c r="R13" s="2">
+      <c r="R13" s="1">
         <f t="shared" si="2"/>
         <v>3.0215717364983892</v>
       </c>
@@ -3063,7 +3059,7 @@
       </c>
     </row>
     <row r="14" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="D14">
+      <c r="D14" s="2">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
@@ -3325,7 +3321,7 @@
       </c>
     </row>
     <row r="15" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="D15">
+      <c r="D15" s="2">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
@@ -3587,7 +3583,7 @@
       </c>
     </row>
     <row r="16" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="D16">
+      <c r="D16" s="2">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
@@ -3849,7 +3845,7 @@
       </c>
     </row>
     <row r="17" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D17">
+      <c r="D17" s="2">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
@@ -4111,7 +4107,7 @@
       </c>
     </row>
     <row r="18" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D18">
+      <c r="D18" s="2">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
@@ -4373,7 +4369,7 @@
       </c>
     </row>
     <row r="19" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D19">
+      <c r="D19" s="2">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
@@ -4635,7 +4631,7 @@
       </c>
     </row>
     <row r="20" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D20">
+      <c r="D20" s="2">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
@@ -4897,7 +4893,7 @@
       </c>
     </row>
     <row r="21" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D21">
+      <c r="D21" s="2">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
@@ -4953,7 +4949,7 @@
         <f t="shared" si="2"/>
         <v>3.9766905763089362</v>
       </c>
-      <c r="R21" s="2">
+      <c r="R21" s="1">
         <f t="shared" si="2"/>
         <v>4.1132568023006373</v>
       </c>
@@ -5159,7 +5155,7 @@
       </c>
     </row>
     <row r="22" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D22">
+      <c r="D22" s="2">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
@@ -5421,7 +5417,7 @@
       </c>
     </row>
     <row r="23" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D23">
+      <c r="D23" s="2">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
@@ -5683,7 +5679,7 @@
       </c>
     </row>
     <row r="24" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D24">
+      <c r="D24" s="2">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
@@ -5945,7 +5941,7 @@
       </c>
     </row>
     <row r="25" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D25">
+      <c r="D25" s="2">
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
@@ -6207,7 +6203,7 @@
       </c>
     </row>
     <row r="26" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D26">
+      <c r="D26" s="2">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
@@ -6469,7 +6465,7 @@
       </c>
     </row>
     <row r="27" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D27">
+      <c r="D27" s="2">
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
@@ -6731,7 +6727,7 @@
       </c>
     </row>
     <row r="28" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D28">
+      <c r="D28" s="2">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
@@ -6993,7 +6989,7 @@
       </c>
     </row>
     <row r="29" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D29">
+      <c r="D29" s="2">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
@@ -7255,7 +7251,7 @@
       </c>
     </row>
     <row r="30" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D30">
+      <c r="D30" s="2">
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
@@ -7517,7 +7513,7 @@
       </c>
     </row>
     <row r="31" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D31">
+      <c r="D31" s="2">
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
@@ -7779,7 +7775,7 @@
       </c>
     </row>
     <row r="32" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D32">
+      <c r="D32" s="2">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
@@ -8041,7 +8037,7 @@
       </c>
     </row>
     <row r="33" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D33">
+      <c r="D33" s="2">
         <f t="shared" si="3"/>
         <v>29</v>
       </c>
@@ -8303,7 +8299,7 @@
       </c>
     </row>
     <row r="34" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D34">
+      <c r="D34" s="2">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
@@ -8565,7 +8561,7 @@
       </c>
     </row>
     <row r="35" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D35">
+      <c r="D35" s="2">
         <f t="shared" si="3"/>
         <v>31</v>
       </c>
@@ -8621,7 +8617,7 @@
         <f t="shared" si="12"/>
         <v>4.9789702495073911</v>
       </c>
-      <c r="R35" s="3">
+      <c r="R35" s="1">
         <f t="shared" si="12"/>
         <v>5.144494908497216</v>
       </c>
@@ -8827,7 +8823,7 @@
       </c>
     </row>
     <row r="36" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D36">
+      <c r="D36" s="2">
         <f t="shared" si="3"/>
         <v>32</v>
       </c>
@@ -9089,7 +9085,7 @@
       </c>
     </row>
     <row r="37" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D37">
+      <c r="D37" s="2">
         <f t="shared" si="3"/>
         <v>33</v>
       </c>
@@ -9141,7 +9137,7 @@
         <f t="shared" si="12"/>
         <v>4.9012386739869926</v>
       </c>
-      <c r="Q37" s="2">
+      <c r="Q37" s="1">
         <f t="shared" si="12"/>
         <v>5.0832738603848062</v>
       </c>
@@ -9351,7 +9347,7 @@
       </c>
     </row>
     <row r="38" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D38">
+      <c r="D38" s="2">
         <f t="shared" si="3"/>
         <v>34</v>
       </c>
@@ -9613,7 +9609,7 @@
       </c>
     </row>
     <row r="39" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D39">
+      <c r="D39" s="2">
         <f t="shared" si="3"/>
         <v>35</v>
       </c>
@@ -9875,7 +9871,7 @@
       </c>
     </row>
     <row r="40" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D40">
+      <c r="D40" s="2">
         <f t="shared" si="3"/>
         <v>36</v>
       </c>
@@ -10137,7 +10133,7 @@
       </c>
     </row>
     <row r="41" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D41">
+      <c r="D41" s="2">
         <f t="shared" si="3"/>
         <v>37</v>
       </c>
@@ -10399,7 +10395,7 @@
       </c>
     </row>
     <row r="42" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D42">
+      <c r="D42" s="2">
         <f t="shared" si="3"/>
         <v>38</v>
       </c>
@@ -10661,7 +10657,7 @@
       </c>
     </row>
     <row r="43" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D43">
+      <c r="D43" s="2">
         <f t="shared" si="3"/>
         <v>39</v>
       </c>
@@ -10923,7 +10919,7 @@
       </c>
     </row>
     <row r="44" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D44">
+      <c r="D44" s="2">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
@@ -11185,7 +11181,7 @@
       </c>
     </row>
     <row r="45" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D45">
+      <c r="D45" s="2">
         <f t="shared" si="3"/>
         <v>41</v>
       </c>
@@ -11447,7 +11443,7 @@
       </c>
     </row>
     <row r="46" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D46">
+      <c r="D46" s="2">
         <f t="shared" si="3"/>
         <v>42</v>
       </c>
@@ -11709,7 +11705,7 @@
       </c>
     </row>
     <row r="47" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D47">
+      <c r="D47" s="2">
         <f t="shared" si="3"/>
         <v>43</v>
       </c>
@@ -11971,7 +11967,7 @@
       </c>
     </row>
     <row r="48" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D48">
+      <c r="D48" s="2">
         <f t="shared" si="3"/>
         <v>44</v>
       </c>
@@ -12233,7 +12229,7 @@
       </c>
     </row>
     <row r="49" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D49">
+      <c r="D49" s="2">
         <f t="shared" si="3"/>
         <v>45</v>
       </c>
@@ -12495,7 +12491,7 @@
       </c>
     </row>
     <row r="50" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D50">
+      <c r="D50" s="2">
         <f t="shared" si="3"/>
         <v>46</v>
       </c>
@@ -12757,7 +12753,7 @@
       </c>
     </row>
     <row r="51" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D51">
+      <c r="D51" s="2">
         <f t="shared" si="3"/>
         <v>47</v>
       </c>
@@ -13019,7 +13015,7 @@
       </c>
     </row>
     <row r="52" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D52">
+      <c r="D52" s="2">
         <f t="shared" si="3"/>
         <v>48</v>
       </c>
@@ -13281,7 +13277,7 @@
       </c>
     </row>
     <row r="53" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D53">
+      <c r="D53" s="2">
         <f t="shared" si="3"/>
         <v>49</v>
       </c>
@@ -13543,7 +13539,7 @@
       </c>
     </row>
     <row r="54" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D54">
+      <c r="D54" s="2">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
@@ -13805,7 +13801,7 @@
       </c>
     </row>
     <row r="55" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D55">
+      <c r="D55" s="2">
         <f t="shared" si="3"/>
         <v>51</v>
       </c>
@@ -14067,7 +14063,7 @@
       </c>
     </row>
     <row r="56" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D56">
+      <c r="D56" s="2">
         <f t="shared" si="3"/>
         <v>52</v>
       </c>
@@ -14329,7 +14325,7 @@
       </c>
     </row>
     <row r="57" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D57">
+      <c r="D57" s="2">
         <f t="shared" si="3"/>
         <v>53</v>
       </c>
@@ -14591,7 +14587,7 @@
       </c>
     </row>
     <row r="58" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D58">
+      <c r="D58" s="2">
         <f t="shared" si="3"/>
         <v>54</v>
       </c>
@@ -14853,7 +14849,7 @@
       </c>
     </row>
     <row r="59" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D59">
+      <c r="D59" s="2">
         <f t="shared" si="3"/>
         <v>55</v>
       </c>
@@ -15115,7 +15111,7 @@
       </c>
     </row>
     <row r="60" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D60">
+      <c r="D60" s="2">
         <f t="shared" si="3"/>
         <v>56</v>
       </c>
@@ -15377,7 +15373,7 @@
       </c>
     </row>
     <row r="61" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D61">
+      <c r="D61" s="2">
         <f t="shared" si="3"/>
         <v>57</v>
       </c>
@@ -15639,7 +15635,7 @@
       </c>
     </row>
     <row r="62" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D62">
+      <c r="D62" s="2">
         <f t="shared" si="3"/>
         <v>58</v>
       </c>
@@ -15901,7 +15897,7 @@
       </c>
     </row>
     <row r="63" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D63">
+      <c r="D63" s="2">
         <f t="shared" si="3"/>
         <v>59</v>
       </c>
@@ -16163,7 +16159,7 @@
       </c>
     </row>
     <row r="64" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D64">
+      <c r="D64" s="2">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
@@ -16425,7 +16421,7 @@
       </c>
     </row>
     <row r="65" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D65">
+      <c r="D65" s="2">
         <f t="shared" si="3"/>
         <v>61</v>
       </c>
@@ -16687,7 +16683,7 @@
       </c>
     </row>
     <row r="66" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D66">
+      <c r="D66" s="2">
         <f t="shared" si="3"/>
         <v>62</v>
       </c>
@@ -16949,7 +16945,7 @@
       </c>
     </row>
     <row r="67" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D67">
+      <c r="D67" s="2">
         <f t="shared" si="3"/>
         <v>63</v>
       </c>
@@ -17211,7 +17207,7 @@
       </c>
     </row>
     <row r="68" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D68">
+      <c r="D68" s="2">
         <f t="shared" si="3"/>
         <v>64</v>
       </c>
@@ -17473,7 +17469,7 @@
       </c>
     </row>
     <row r="69" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D69">
+      <c r="D69" s="2">
         <f t="shared" si="3"/>
         <v>65</v>
       </c>
@@ -17735,7 +17731,7 @@
       </c>
     </row>
     <row r="70" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D70">
+      <c r="D70" s="2">
         <f t="shared" si="3"/>
         <v>66</v>
       </c>
@@ -17997,7 +17993,7 @@
       </c>
     </row>
     <row r="71" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D71">
+      <c r="D71" s="2">
         <f t="shared" si="3"/>
         <v>67</v>
       </c>
@@ -18259,7 +18255,7 @@
       </c>
     </row>
     <row r="72" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D72">
+      <c r="D72" s="2">
         <f t="shared" si="3"/>
         <v>68</v>
       </c>
@@ -18521,7 +18517,7 @@
       </c>
     </row>
     <row r="73" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D73">
+      <c r="D73" s="2">
         <f t="shared" ref="D73:D132" si="28">D72 + 1</f>
         <v>69</v>
       </c>
@@ -18783,7 +18779,7 @@
       </c>
     </row>
     <row r="74" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D74">
+      <c r="D74" s="2">
         <f t="shared" si="28"/>
         <v>70</v>
       </c>
@@ -19045,7 +19041,7 @@
       </c>
     </row>
     <row r="75" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D75">
+      <c r="D75" s="2">
         <f t="shared" si="28"/>
         <v>71</v>
       </c>
@@ -19307,7 +19303,7 @@
       </c>
     </row>
     <row r="76" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D76">
+      <c r="D76" s="2">
         <f t="shared" si="28"/>
         <v>72</v>
       </c>
@@ -19569,7 +19565,7 @@
       </c>
     </row>
     <row r="77" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D77">
+      <c r="D77" s="2">
         <f t="shared" si="28"/>
         <v>73</v>
       </c>
@@ -19831,7 +19827,7 @@
       </c>
     </row>
     <row r="78" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D78">
+      <c r="D78" s="2">
         <f t="shared" si="28"/>
         <v>74</v>
       </c>
@@ -20093,7 +20089,7 @@
       </c>
     </row>
     <row r="79" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D79">
+      <c r="D79" s="2">
         <f t="shared" si="28"/>
         <v>75</v>
       </c>
@@ -20355,7 +20351,7 @@
       </c>
     </row>
     <row r="80" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D80">
+      <c r="D80" s="2">
         <f t="shared" si="28"/>
         <v>76</v>
       </c>
@@ -20617,7 +20613,7 @@
       </c>
     </row>
     <row r="81" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D81">
+      <c r="D81" s="2">
         <f t="shared" si="28"/>
         <v>77</v>
       </c>
@@ -20879,7 +20875,7 @@
       </c>
     </row>
     <row r="82" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D82">
+      <c r="D82" s="2">
         <f t="shared" si="28"/>
         <v>78</v>
       </c>
@@ -21141,7 +21137,7 @@
       </c>
     </row>
     <row r="83" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D83">
+      <c r="D83" s="2">
         <f t="shared" si="28"/>
         <v>79</v>
       </c>
@@ -21403,7 +21399,7 @@
       </c>
     </row>
     <row r="84" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D84">
+      <c r="D84" s="2">
         <f t="shared" si="28"/>
         <v>80</v>
       </c>
@@ -21665,7 +21661,7 @@
       </c>
     </row>
     <row r="85" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D85">
+      <c r="D85" s="2">
         <f t="shared" si="28"/>
         <v>81</v>
       </c>
@@ -21927,7 +21923,7 @@
       </c>
     </row>
     <row r="86" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D86">
+      <c r="D86" s="2">
         <f t="shared" si="28"/>
         <v>82</v>
       </c>
@@ -22189,7 +22185,7 @@
       </c>
     </row>
     <row r="87" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D87">
+      <c r="D87" s="2">
         <f t="shared" si="28"/>
         <v>83</v>
       </c>
@@ -22451,7 +22447,7 @@
       </c>
     </row>
     <row r="88" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D88">
+      <c r="D88" s="2">
         <f t="shared" si="28"/>
         <v>84</v>
       </c>
@@ -22713,7 +22709,7 @@
       </c>
     </row>
     <row r="89" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D89">
+      <c r="D89" s="2">
         <f t="shared" si="28"/>
         <v>85</v>
       </c>
@@ -22975,7 +22971,7 @@
       </c>
     </row>
     <row r="90" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D90">
+      <c r="D90" s="2">
         <f t="shared" si="28"/>
         <v>86</v>
       </c>
@@ -23237,7 +23233,7 @@
       </c>
     </row>
     <row r="91" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D91">
+      <c r="D91" s="2">
         <f t="shared" si="28"/>
         <v>87</v>
       </c>
@@ -23499,7 +23495,7 @@
       </c>
     </row>
     <row r="92" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D92">
+      <c r="D92" s="2">
         <f t="shared" si="28"/>
         <v>88</v>
       </c>
@@ -23761,7 +23757,7 @@
       </c>
     </row>
     <row r="93" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D93">
+      <c r="D93" s="2">
         <f t="shared" si="28"/>
         <v>89</v>
       </c>
@@ -24023,7 +24019,7 @@
       </c>
     </row>
     <row r="94" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D94">
+      <c r="D94" s="2">
         <f t="shared" si="28"/>
         <v>90</v>
       </c>
@@ -24285,7 +24281,7 @@
       </c>
     </row>
     <row r="95" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D95">
+      <c r="D95" s="2">
         <f t="shared" si="28"/>
         <v>91</v>
       </c>
@@ -24547,7 +24543,7 @@
       </c>
     </row>
     <row r="96" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D96">
+      <c r="D96" s="2">
         <f t="shared" si="28"/>
         <v>92</v>
       </c>
@@ -24809,7 +24805,7 @@
       </c>
     </row>
     <row r="97" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D97">
+      <c r="D97" s="2">
         <f t="shared" si="28"/>
         <v>93</v>
       </c>
@@ -25071,7 +25067,7 @@
       </c>
     </row>
     <row r="98" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D98">
+      <c r="D98" s="2">
         <f t="shared" si="28"/>
         <v>94</v>
       </c>
@@ -25333,7 +25329,7 @@
       </c>
     </row>
     <row r="99" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D99">
+      <c r="D99" s="2">
         <f t="shared" si="28"/>
         <v>95</v>
       </c>
@@ -25595,7 +25591,7 @@
       </c>
     </row>
     <row r="100" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D100">
+      <c r="D100" s="2">
         <f t="shared" si="28"/>
         <v>96</v>
       </c>
@@ -25857,7 +25853,7 @@
       </c>
     </row>
     <row r="101" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D101">
+      <c r="D101" s="2">
         <f t="shared" si="28"/>
         <v>97</v>
       </c>
@@ -26119,7 +26115,7 @@
       </c>
     </row>
     <row r="102" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D102">
+      <c r="D102" s="2">
         <f t="shared" si="28"/>
         <v>98</v>
       </c>
@@ -26381,7 +26377,7 @@
       </c>
     </row>
     <row r="103" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D103">
+      <c r="D103" s="2">
         <f t="shared" si="28"/>
         <v>99</v>
       </c>
@@ -26643,7 +26639,7 @@
       </c>
     </row>
     <row r="104" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D104">
+      <c r="D104" s="2">
         <f t="shared" si="28"/>
         <v>100</v>
       </c>
@@ -26905,7 +26901,7 @@
       </c>
     </row>
     <row r="105" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D105">
+      <c r="D105" s="2">
         <f t="shared" si="28"/>
         <v>101</v>
       </c>
@@ -27167,7 +27163,7 @@
       </c>
     </row>
     <row r="106" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D106">
+      <c r="D106" s="2">
         <f t="shared" si="28"/>
         <v>102</v>
       </c>
@@ -27429,7 +27425,7 @@
       </c>
     </row>
     <row r="107" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D107">
+      <c r="D107" s="2">
         <f t="shared" si="28"/>
         <v>103</v>
       </c>
@@ -27691,7 +27687,7 @@
       </c>
     </row>
     <row r="108" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D108">
+      <c r="D108" s="2">
         <f t="shared" si="28"/>
         <v>104</v>
       </c>
@@ -27953,7 +27949,7 @@
       </c>
     </row>
     <row r="109" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D109">
+      <c r="D109" s="2">
         <f t="shared" si="28"/>
         <v>105</v>
       </c>
@@ -28215,7 +28211,7 @@
       </c>
     </row>
     <row r="110" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D110">
+      <c r="D110" s="2">
         <f t="shared" si="28"/>
         <v>106</v>
       </c>
@@ -28477,7 +28473,7 @@
       </c>
     </row>
     <row r="111" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D111">
+      <c r="D111" s="2">
         <f t="shared" si="28"/>
         <v>107</v>
       </c>
@@ -28739,7 +28735,7 @@
       </c>
     </row>
     <row r="112" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D112">
+      <c r="D112" s="2">
         <f t="shared" si="28"/>
         <v>108</v>
       </c>
@@ -29001,7 +28997,7 @@
       </c>
     </row>
     <row r="113" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D113">
+      <c r="D113" s="2">
         <f t="shared" si="28"/>
         <v>109</v>
       </c>
@@ -29263,7 +29259,7 @@
       </c>
     </row>
     <row r="114" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D114">
+      <c r="D114" s="2">
         <f t="shared" si="28"/>
         <v>110</v>
       </c>
@@ -29525,7 +29521,7 @@
       </c>
     </row>
     <row r="115" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D115">
+      <c r="D115" s="2">
         <f t="shared" si="28"/>
         <v>111</v>
       </c>
@@ -29787,7 +29783,7 @@
       </c>
     </row>
     <row r="116" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D116">
+      <c r="D116" s="2">
         <f t="shared" si="28"/>
         <v>112</v>
       </c>
@@ -30049,7 +30045,7 @@
       </c>
     </row>
     <row r="117" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D117">
+      <c r="D117" s="2">
         <f t="shared" si="28"/>
         <v>113</v>
       </c>
@@ -30311,7 +30307,7 @@
       </c>
     </row>
     <row r="118" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D118">
+      <c r="D118" s="2">
         <f t="shared" si="28"/>
         <v>114</v>
       </c>
@@ -30573,7 +30569,7 @@
       </c>
     </row>
     <row r="119" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D119">
+      <c r="D119" s="2">
         <f t="shared" si="28"/>
         <v>115</v>
       </c>
@@ -30835,7 +30831,7 @@
       </c>
     </row>
     <row r="120" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D120">
+      <c r="D120" s="2">
         <f t="shared" si="28"/>
         <v>116</v>
       </c>
@@ -31097,7 +31093,7 @@
       </c>
     </row>
     <row r="121" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D121">
+      <c r="D121" s="2">
         <f t="shared" si="28"/>
         <v>117</v>
       </c>
@@ -31359,7 +31355,7 @@
       </c>
     </row>
     <row r="122" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D122">
+      <c r="D122" s="2">
         <f t="shared" si="28"/>
         <v>118</v>
       </c>
@@ -31621,7 +31617,7 @@
       </c>
     </row>
     <row r="123" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D123">
+      <c r="D123" s="2">
         <f t="shared" si="28"/>
         <v>119</v>
       </c>
@@ -31883,7 +31879,7 @@
       </c>
     </row>
     <row r="124" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D124">
+      <c r="D124" s="2">
         <f t="shared" si="28"/>
         <v>120</v>
       </c>
@@ -32145,7 +32141,7 @@
       </c>
     </row>
     <row r="125" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D125">
+      <c r="D125" s="2">
         <f t="shared" si="28"/>
         <v>121</v>
       </c>
@@ -32407,7 +32403,7 @@
       </c>
     </row>
     <row r="126" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D126">
+      <c r="D126" s="2">
         <f t="shared" si="28"/>
         <v>122</v>
       </c>
@@ -32669,7 +32665,7 @@
       </c>
     </row>
     <row r="127" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D127">
+      <c r="D127" s="2">
         <f t="shared" si="28"/>
         <v>123</v>
       </c>
@@ -32931,7 +32927,7 @@
       </c>
     </row>
     <row r="128" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D128">
+      <c r="D128" s="2">
         <f t="shared" si="28"/>
         <v>124</v>
       </c>
@@ -33193,7 +33189,7 @@
       </c>
     </row>
     <row r="129" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D129">
+      <c r="D129" s="2">
         <f t="shared" si="28"/>
         <v>125</v>
       </c>
@@ -33455,7 +33451,7 @@
       </c>
     </row>
     <row r="130" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D130">
+      <c r="D130" s="2">
         <f t="shared" si="28"/>
         <v>126</v>
       </c>
@@ -33717,7 +33713,7 @@
       </c>
     </row>
     <row r="131" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D131">
+      <c r="D131" s="2">
         <f t="shared" si="28"/>
         <v>127</v>
       </c>
@@ -33979,7 +33975,7 @@
       </c>
     </row>
     <row r="132" spans="4:68" x14ac:dyDescent="0.35">
-      <c r="D132">
+      <c r="D132" s="2">
         <f t="shared" si="28"/>
         <v>128</v>
       </c>

</xml_diff>